<commit_message>
Temporary code for DR
</commit_message>
<xml_diff>
--- a/storage/app/imports/JORequestForm.xlsx
+++ b/storage/app/imports/JORequestForm.xlsx
@@ -147,9 +147,6 @@
     <t>Item Description</t>
   </si>
   <si>
-    <t>Department Name</t>
-  </si>
-  <si>
     <t>pc/s</t>
   </si>
   <si>
@@ -198,10 +195,13 @@
     <t>Project/Activity:</t>
   </si>
   <si>
-    <t>Stephine David Severino</t>
-  </si>
-  <si>
     <t>Trial project activity2</t>
+  </si>
+  <si>
+    <t>department11</t>
+  </si>
+  <si>
+    <t>Jonah Faye Benares</t>
   </si>
 </sst>
 </file>
@@ -502,15 +502,162 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -523,15 +670,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -540,144 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,7 +716,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1019,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:K13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,14 +1054,14 @@
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -1069,14 +1069,14 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
@@ -1084,14 +1084,14 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7"/>
@@ -1099,197 +1099,197 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="66"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="64" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
+      <c r="I7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="69">
+      <c r="B8" s="38"/>
+      <c r="C8" s="39">
         <v>45574</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="66"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="70">
+      <c r="I8" s="40">
         <v>45575</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="72"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="75"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="70">
+      <c r="I9" s="40">
         <v>45576</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="77"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="78" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="79"/>
-      <c r="E10" s="80"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="81">
+      <c r="I10" s="51">
         <v>1</v>
       </c>
-      <c r="J10" s="82"/>
-      <c r="K10" s="83"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="87"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="50"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="72"/>
     </row>
     <row r="13" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="55"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="80"/>
       <c r="L13" s="22"/>
     </row>
     <row r="14" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="47"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="13" t="s">
         <v>18</v>
       </c>
@@ -1299,22 +1299,22 @@
       <c r="I15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="44"/>
+      <c r="K15" s="77"/>
     </row>
     <row r="16" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>1</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="52"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="19">
         <v>1</v>
       </c>
@@ -1324,22 +1324,22 @@
       <c r="I16" s="17">
         <v>200</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="59">
         <v>200</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="60"/>
     </row>
     <row r="17" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>2</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="52"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="19">
         <v>1</v>
       </c>
@@ -1349,22 +1349,22 @@
       <c r="I17" s="17">
         <v>300</v>
       </c>
-      <c r="J17" s="37">
+      <c r="J17" s="59">
         <v>300</v>
       </c>
-      <c r="K17" s="38"/>
+      <c r="K17" s="60"/>
     </row>
     <row r="18" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="74"/>
       <c r="G18" s="19">
         <v>1</v>
       </c>
@@ -1374,22 +1374,22 @@
       <c r="I18" s="17">
         <v>400</v>
       </c>
-      <c r="J18" s="37">
+      <c r="J18" s="59">
         <v>400</v>
       </c>
-      <c r="K18" s="38"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>4</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="15">
         <v>1</v>
       </c>
@@ -1399,35 +1399,35 @@
       <c r="I19" s="17">
         <v>500</v>
       </c>
-      <c r="J19" s="37">
+      <c r="J19" s="59">
         <v>500</v>
       </c>
-      <c r="K19" s="38"/>
+      <c r="K19" s="60"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>5</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
+      <c r="B20" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I20" s="17">
         <v>600</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="59">
         <v>600</v>
       </c>
-      <c r="K20" s="38"/>
+      <c r="K20" s="60"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
@@ -1447,13 +1447,13 @@
       <c r="D22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="77"/>
       <c r="J22" s="13" t="s">
         <v>34</v>
       </c>
@@ -1469,18 +1469,18 @@
         <v>1</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="74"/>
       <c r="J23" s="18">
         <v>1</v>
       </c>
@@ -1496,18 +1496,18 @@
         <v>2</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+        <v>43</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="74"/>
       <c r="J24" s="18">
         <v>2</v>
       </c>
@@ -1523,18 +1523,18 @@
         <v>3</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+        <v>44</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="74"/>
       <c r="J25" s="18">
         <v>3</v>
       </c>
@@ -1550,18 +1550,18 @@
         <v>4</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+        <v>45</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="74"/>
       <c r="J26" s="16">
         <v>4</v>
       </c>
@@ -1573,21 +1573,45 @@
       <c r="A27" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
+      <c r="B27" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="I7:K7"/>
@@ -1604,30 +1628,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DR, PO, and other fixes
</commit_message>
<xml_diff>
--- a/storage/app/imports/JORequestForm.xlsx
+++ b/storage/app/imports/JORequestForm.xlsx
@@ -120,9 +120,6 @@
 Size: 77cmx208cm.</t>
   </si>
   <si>
-    <t>ADM-137-2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">General Description: </t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Jonah Faye Benares</t>
+  </si>
+  <si>
+    <t>ADM-137-20241</t>
   </si>
 </sst>
 </file>
@@ -499,6 +499,57 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,124 +568,73 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N22" sqref="M21:N22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,14 +1039,14 @@
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -1054,14 +1054,14 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
@@ -1069,14 +1069,14 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7"/>
@@ -1084,131 +1084,133 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="74"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="48"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="48"/>
+      <c r="I7" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51">
-        <v>45574</v>
-      </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40">
+        <v>45663</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="52">
-        <v>45575</v>
-      </c>
-      <c r="J8" s="53"/>
-      <c r="K8" s="54"/>
+      <c r="I8" s="43">
+        <v>45297</v>
+      </c>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="52">
-        <v>45576</v>
-      </c>
-      <c r="J9" s="53"/>
-      <c r="K9" s="54"/>
+      <c r="I9" s="43">
+        <v>45298</v>
+      </c>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="69"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
+      <c r="I10" s="71">
+        <v>1</v>
+      </c>
+      <c r="J10" s="72"/>
+      <c r="K10" s="73"/>
     </row>
     <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="68"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
@@ -1229,10 +1231,10 @@
     </row>
     <row r="13" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="81" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="81" t="s">
-        <v>53</v>
       </c>
       <c r="C13" s="82"/>
       <c r="D13" s="82"/>
@@ -1247,7 +1249,7 @@
     </row>
     <row r="14" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="75" t="s">
         <v>23</v>
@@ -1266,13 +1268,13 @@
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48"/>
       <c r="G15" s="13" t="s">
         <v>18</v>
       </c>
@@ -1287,13 +1289,13 @@
       <c r="A16" s="18">
         <v>1</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51"/>
       <c r="G16" s="19">
         <v>1</v>
       </c>
@@ -1308,13 +1310,13 @@
       <c r="A17" s="18">
         <v>2</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="51"/>
       <c r="G17" s="19">
         <v>1</v>
       </c>
@@ -1329,13 +1331,13 @@
       <c r="A18" s="18">
         <v>3</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
       <c r="G18" s="19">
         <v>1</v>
       </c>
@@ -1350,13 +1352,13 @@
       <c r="A19" s="14">
         <v>4</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="15">
         <v>1</v>
       </c>
@@ -1371,18 +1373,18 @@
       <c r="A20" s="14">
         <v>5</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
+      <c r="B20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" s="17">
         <v>600.32000000000005</v>
@@ -1390,7 +1392,7 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,20 +1406,20 @@
         <v>19</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="13" t="s">
+      <c r="K22" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1428,18 +1430,18 @@
         <v>1</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
       <c r="J23" s="18">
         <v>5</v>
       </c>
@@ -1453,18 +1455,18 @@
         <v>2</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
+        <v>41</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
       <c r="J24" s="18">
         <v>6</v>
       </c>
@@ -1478,18 +1480,18 @@
         <v>3</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
+        <v>42</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
       <c r="J25" s="18">
         <v>7</v>
       </c>
@@ -1503,18 +1505,18 @@
         <v>4</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
       <c r="J26" s="16">
         <v>4</v>
       </c>
@@ -1522,20 +1524,20 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -1547,22 +1549,19 @@
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="E23:I23"/>
     <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="I8:K8"/>
@@ -1570,9 +1569,12 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix Errors and update PR template
</commit_message>
<xml_diff>
--- a/storage/app/imports/JORequestForm.xlsx
+++ b/storage/app/imports/JORequestForm.xlsx
@@ -198,7 +198,7 @@
     <t>Jonah Faye Benares</t>
   </si>
   <si>
-    <t>ADM-137-20241112</t>
+    <t>ADM-137-20241112awa</t>
   </si>
 </sst>
 </file>
@@ -1189,9 +1189,7 @@
       <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="71">
-        <v>1</v>
-      </c>
+      <c r="I10" s="71"/>
       <c r="J10" s="72"/>
       <c r="K10" s="73"/>
     </row>

</xml_diff>

<commit_message>
Fix error of DR
</commit_message>
<xml_diff>
--- a/storage/app/imports/JORequestForm.xlsx
+++ b/storage/app/imports/JORequestForm.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -198,10 +198,7 @@
     <t>Jonah Faye Benares</t>
   </si>
   <si>
-    <t>ADM-137-20241112awaw</t>
-  </si>
-  <si>
-    <t>aka</t>
+    <t>ADM-137-20242025</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,8 +1294,8 @@
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="19" t="s">
-        <v>56</v>
+      <c r="G16" s="19">
+        <v>1</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>21</v>

</xml_diff>